<commit_message>
The config Excel importer now handles updates in the spreadsheet and updates the database.
</commit_message>
<xml_diff>
--- a/ModelCatalogueCorePluginTestApp/test/integration/resources/org/modelcatalogue/integration/excel/loinc.xlsx
+++ b/ModelCatalogueCorePluginTestApp/test/integration/resources/org/modelcatalogue/integration/excel/loinc.xlsx
@@ -884,7 +884,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomLeft" activeCell="AF11" sqref="AF11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -896,7 +896,7 @@
     <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.75" customWidth="1"/>
     <col min="9" max="9" width="8.375" customWidth="1"/>
     <col min="10" max="10" width="10.75" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.75" customWidth="1"/>

</xml_diff>